<commit_message>
Tes commit setelah perpanjang key
</commit_message>
<xml_diff>
--- a/output/2025/EFISIENSI PER DINAS.xlsx
+++ b/output/2025/EFISIENSI PER DINAS.xlsx
@@ -2110,19 +2110,19 @@
         <v>17122820</v>
       </c>
       <c r="BB4" s="4">
-        <v>26342800</v>
+        <v>17122000</v>
       </c>
       <c r="BC4" s="4">
-        <v>9219980</v>
+        <v>-820</v>
       </c>
       <c r="BD4" s="4">
-        <v>0</v>
+        <v>100.00889372861981</v>
       </c>
       <c r="BE4" s="4">
         <v>23750600</v>
       </c>
       <c r="BF4" s="4">
-        <v>0</v>
+        <v>9220800</v>
       </c>
       <c r="BG4" s="4">
         <v>12968500</v>
@@ -2134,19 +2134,19 @@
         <v>8429525</v>
       </c>
       <c r="BJ4" s="4">
-        <v>12968500</v>
+        <v>8380000</v>
       </c>
       <c r="BK4" s="4">
-        <v>4538975</v>
+        <v>-49525</v>
       </c>
       <c r="BL4" s="4">
-        <v>0</v>
+        <v>101.09110537070593</v>
       </c>
       <c r="BM4" s="4">
         <v>6090000</v>
       </c>
       <c r="BN4" s="4">
-        <v>0</v>
+        <v>4588500</v>
       </c>
       <c r="BO4" s="4">
         <v>10238000</v>
@@ -2158,19 +2158,19 @@
         <v>6654700</v>
       </c>
       <c r="BR4" s="4">
-        <v>10238000</v>
+        <v>6603000</v>
       </c>
       <c r="BS4" s="4">
-        <v>3583300</v>
+        <v>-51700</v>
       </c>
       <c r="BT4" s="4">
-        <v>0</v>
+        <v>101.44280411910809</v>
       </c>
       <c r="BU4" s="4">
         <v>5751600</v>
       </c>
       <c r="BV4" s="4">
-        <v>0</v>
+        <v>3635000</v>
       </c>
       <c r="CM4" s="4">
         <v>28000000</v>
@@ -2182,19 +2182,19 @@
         <v>18200000</v>
       </c>
       <c r="CP4" s="4">
-        <v>28000000</v>
+        <v>18200000</v>
       </c>
       <c r="CQ4" s="4">
-        <v>9800000</v>
+        <v>0</v>
       </c>
       <c r="CR4" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="CS4" s="4">
         <v>5040000</v>
       </c>
       <c r="CT4" s="4">
-        <v>0</v>
+        <v>9800000</v>
       </c>
       <c r="EA4" s="4">
         <v>32013200</v>
@@ -2206,19 +2206,19 @@
         <v>20808580</v>
       </c>
       <c r="ED4" s="4">
-        <v>32013200</v>
+        <v>24330000</v>
       </c>
       <c r="EE4" s="4">
-        <v>11204620</v>
+        <v>3521420</v>
       </c>
       <c r="EF4" s="4">
-        <v>0</v>
+        <v>68.57171416790574</v>
       </c>
       <c r="EG4" s="4">
         <v>0</v>
       </c>
       <c r="EH4" s="4">
-        <v>0</v>
+        <v>7683200</v>
       </c>
       <c r="EY4" s="4">
         <v>131289181156</v>
@@ -2230,10 +2230,10 @@
         <v>131289181156</v>
       </c>
       <c r="FB4" s="4">
-        <v>131289181156</v>
+        <v>131281739356</v>
       </c>
       <c r="FC4" s="4">
-        <v>0</v>
+        <v>-7441800</v>
       </c>
       <c r="FD4" s="4">
         <v>0</v>
@@ -2242,7 +2242,7 @@
         <v>59311386558</v>
       </c>
       <c r="FF4" s="4">
-        <v>0</v>
+        <v>7441800</v>
       </c>
       <c r="FG4" s="4">
         <v>131509513656</v>
@@ -2254,19 +2254,19 @@
         <v>131415781781</v>
       </c>
       <c r="FJ4" s="4">
-        <v>131462076656</v>
+        <v>131419707356</v>
       </c>
       <c r="FK4" s="4">
-        <v>46294875</v>
+        <v>3925575</v>
       </c>
       <c r="FL4" s="4">
-        <v>50.60925112188357</v>
+        <v>95.8119103026585</v>
       </c>
       <c r="FM4" s="4">
         <v>72330200</v>
       </c>
       <c r="FN4" s="4">
-        <v>47437000</v>
+        <v>89806300</v>
       </c>
       <c r="FO4" s="4">
         <v>811615000</v>
@@ -2278,19 +2278,19 @@
         <v>405807500</v>
       </c>
       <c r="FR4" s="4">
-        <v>415042000</v>
+        <v>460007000</v>
       </c>
       <c r="FS4" s="4">
-        <v>9234500</v>
+        <v>54199500</v>
       </c>
       <c r="FT4" s="4">
-        <v>97.72441366904259</v>
+        <v>86.64403688941185</v>
       </c>
       <c r="FU4" s="4">
         <v>31698000</v>
       </c>
       <c r="FV4" s="4">
-        <v>396573000</v>
+        <v>351608000</v>
       </c>
       <c r="FW4" s="4">
         <v>160098000</v>
@@ -2302,19 +2302,19 @@
         <v>80049000</v>
       </c>
       <c r="FZ4" s="4">
-        <v>64583000</v>
+        <v>61163000</v>
       </c>
       <c r="GA4" s="4">
-        <v>-15466000</v>
+        <v>-18886000</v>
       </c>
       <c r="GB4" s="4">
-        <v>119.32066609201864</v>
+        <v>123.59304925732988</v>
       </c>
       <c r="GC4" s="4">
         <v>17967000</v>
       </c>
       <c r="GD4" s="4">
-        <v>95515000</v>
+        <v>98935000</v>
       </c>
       <c r="GE4" s="4">
         <v>2143600000</v>
@@ -2326,19 +2326,19 @@
         <v>1071800000</v>
       </c>
       <c r="GH4" s="4">
-        <v>1593250000</v>
+        <v>1170850000</v>
       </c>
       <c r="GI4" s="4">
-        <v>521450000</v>
+        <v>99050000</v>
       </c>
       <c r="GJ4" s="4">
-        <v>51.34819929091249</v>
+        <v>90.75853704049263</v>
       </c>
       <c r="GK4" s="4">
         <v>207161000</v>
       </c>
       <c r="GL4" s="4">
-        <v>550350000</v>
+        <v>972750000</v>
       </c>
       <c r="GU4" s="4">
         <v>51111000</v>
@@ -2350,19 +2350,19 @@
         <v>25555500</v>
       </c>
       <c r="GX4" s="4">
+        <v>0</v>
+      </c>
+      <c r="GY4" s="4">
+        <v>-25555500</v>
+      </c>
+      <c r="GZ4" s="4">
+        <v>200</v>
+      </c>
+      <c r="HA4" s="4">
+        <v>0</v>
+      </c>
+      <c r="HB4" s="4">
         <v>51111000</v>
-      </c>
-      <c r="GY4" s="4">
-        <v>25555500</v>
-      </c>
-      <c r="GZ4" s="4">
-        <v>0</v>
-      </c>
-      <c r="HA4" s="4">
-        <v>0</v>
-      </c>
-      <c r="HB4" s="4">
-        <v>0</v>
       </c>
       <c r="HK4" s="4">
         <v>119140400</v>
@@ -2374,19 +2374,19 @@
         <v>77441260</v>
       </c>
       <c r="HN4" s="4">
-        <v>93333000</v>
+        <v>72400400</v>
       </c>
       <c r="HO4" s="4">
-        <v>15891740</v>
+        <v>-5040860</v>
       </c>
       <c r="HP4" s="4">
-        <v>61.88952577918874</v>
+        <v>112.08864259550677</v>
       </c>
       <c r="HQ4" s="4">
         <v>23750600</v>
       </c>
       <c r="HR4" s="4">
-        <v>25807400</v>
+        <v>46740000</v>
       </c>
       <c r="HS4" s="4">
         <v>29096200</v>
@@ -2398,19 +2398,19 @@
         <v>18912530</v>
       </c>
       <c r="HV4" s="4">
-        <v>23496300</v>
+        <v>14128500</v>
       </c>
       <c r="HW4" s="4">
-        <v>4583770</v>
+        <v>-4784030</v>
       </c>
       <c r="HX4" s="4">
-        <v>54.98901672972514</v>
+        <v>146.97746490214234</v>
       </c>
       <c r="HY4" s="4">
         <v>6090000</v>
       </c>
       <c r="HZ4" s="4">
-        <v>5599900</v>
+        <v>14967700</v>
       </c>
       <c r="II4" s="4">
         <v>230530000</v>
@@ -2422,19 +2422,19 @@
         <v>149844500</v>
       </c>
       <c r="IL4" s="4">
-        <v>5530000</v>
+        <v>0</v>
       </c>
       <c r="IM4" s="4">
-        <v>-144314500</v>
+        <v>-149844500</v>
       </c>
       <c r="IN4" s="4">
-        <v>278.86051397091177</v>
+        <v>285.7142857142857</v>
       </c>
       <c r="IO4" s="4">
         <v>0</v>
       </c>
       <c r="IP4" s="4">
-        <v>225000000</v>
+        <v>230530000</v>
       </c>
       <c r="IQ4" s="4">
         <v>758120000</v>
@@ -2446,19 +2446,19 @@
         <v>492778000</v>
       </c>
       <c r="IT4" s="4">
-        <v>607420000</v>
+        <v>543580000</v>
       </c>
       <c r="IU4" s="4">
-        <v>114642000</v>
+        <v>50802000</v>
       </c>
       <c r="IV4" s="4">
-        <v>56.794627311168234</v>
+        <v>80.85414295512962</v>
       </c>
       <c r="IW4" s="4">
         <v>77220000</v>
       </c>
       <c r="IX4" s="4">
-        <v>150700000</v>
+        <v>214540000</v>
       </c>
       <c r="JG4" s="4">
         <v>31054970600</v>
@@ -2470,10 +2470,10 @@
         <v>31054970600</v>
       </c>
       <c r="JJ4" s="4">
-        <v>30938696700</v>
+        <v>30919680700</v>
       </c>
       <c r="JK4" s="4">
-        <v>-116273900</v>
+        <v>-135289900</v>
       </c>
       <c r="JL4" s="4">
         <v>0</v>
@@ -2482,7 +2482,7 @@
         <v>45856137793</v>
       </c>
       <c r="JN4" s="4">
-        <v>116273900</v>
+        <v>135289900</v>
       </c>
       <c r="JO4" s="4">
         <v>45733281200</v>
@@ -2494,19 +2494,19 @@
         <v>40639658890</v>
       </c>
       <c r="JR4" s="4">
-        <v>41127462000</v>
+        <v>40546809600</v>
       </c>
       <c r="JS4" s="4">
-        <v>487803110</v>
+        <v>-92849290</v>
       </c>
       <c r="JT4" s="4">
-        <v>90.4232571574393</v>
+        <v>101.82285384249465</v>
       </c>
       <c r="JU4" s="4">
         <v>2563886600</v>
       </c>
       <c r="JV4" s="4">
-        <v>4605819200</v>
+        <v>5186471600</v>
       </c>
       <c r="JW4" s="4">
         <v>922385000</v>
@@ -2518,19 +2518,19 @@
         <v>461192500</v>
       </c>
       <c r="JZ4" s="4">
-        <v>478375000</v>
+        <v>523340000</v>
       </c>
       <c r="KA4" s="4">
-        <v>17182500</v>
+        <v>62147500</v>
       </c>
       <c r="KB4" s="4">
-        <v>96.27433230158773</v>
+        <v>86.52460740363297</v>
       </c>
       <c r="KC4" s="4">
         <v>31698000</v>
       </c>
       <c r="KD4" s="4">
-        <v>444010000</v>
+        <v>399045000</v>
       </c>
       <c r="KE4" s="4">
         <v>160098000</v>
@@ -2542,19 +2542,19 @@
         <v>80049000</v>
       </c>
       <c r="KH4" s="4">
-        <v>64583000</v>
+        <v>61163000</v>
       </c>
       <c r="KI4" s="4">
-        <v>-15466000</v>
+        <v>-18886000</v>
       </c>
       <c r="KJ4" s="4">
-        <v>119.32066609201864</v>
+        <v>123.59304925732988</v>
       </c>
       <c r="KK4" s="4">
         <v>17967000</v>
       </c>
       <c r="KL4" s="4">
-        <v>95515000</v>
+        <v>98935000</v>
       </c>
       <c r="KM4" s="4">
         <v>2143600000</v>
@@ -2566,19 +2566,19 @@
         <v>1071800000</v>
       </c>
       <c r="KP4" s="4">
-        <v>1593250000</v>
+        <v>1170850000</v>
       </c>
       <c r="KQ4" s="4">
-        <v>521450000</v>
+        <v>99050000</v>
       </c>
       <c r="KR4" s="4">
-        <v>51.34819929091249</v>
+        <v>90.75853704049263</v>
       </c>
       <c r="KS4" s="4">
         <v>207161000</v>
       </c>
       <c r="KT4" s="4">
-        <v>550350000</v>
+        <v>972750000</v>
       </c>
       <c r="LC4" s="4">
         <v>51111000</v>
@@ -2590,19 +2590,19 @@
         <v>25555500</v>
       </c>
       <c r="LF4" s="4">
+        <v>0</v>
+      </c>
+      <c r="LG4" s="4">
+        <v>-25555500</v>
+      </c>
+      <c r="LH4" s="4">
+        <v>200</v>
+      </c>
+      <c r="LI4" s="4">
+        <v>0</v>
+      </c>
+      <c r="LJ4" s="4">
         <v>51111000</v>
-      </c>
-      <c r="LG4" s="4">
-        <v>25555500</v>
-      </c>
-      <c r="LH4" s="4">
-        <v>0</v>
-      </c>
-      <c r="LI4" s="4">
-        <v>0</v>
-      </c>
-      <c r="LJ4" s="4">
-        <v>0</v>
       </c>
       <c r="LS4" s="4">
         <v>145483200</v>
@@ -2614,19 +2614,19 @@
         <v>94564080</v>
       </c>
       <c r="LV4" s="4">
-        <v>119675800</v>
+        <v>89522400</v>
       </c>
       <c r="LW4" s="4">
-        <v>25111720</v>
+        <v>-5041680</v>
       </c>
       <c r="LX4" s="4">
-        <v>50.6831225677113</v>
+        <v>109.90134943416147</v>
       </c>
       <c r="LY4" s="4">
         <v>23750600</v>
       </c>
       <c r="LZ4" s="4">
-        <v>25807400</v>
+        <v>55960800</v>
       </c>
       <c r="MA4" s="4">
         <v>42064700</v>
@@ -2638,19 +2638,19 @@
         <v>27342055</v>
       </c>
       <c r="MD4" s="4">
-        <v>36464800</v>
+        <v>22508500</v>
       </c>
       <c r="ME4" s="4">
-        <v>9122745</v>
+        <v>-4833555</v>
       </c>
       <c r="MF4" s="4">
-        <v>38.03596432570371</v>
+        <v>132.83075153955016</v>
       </c>
       <c r="MG4" s="4">
         <v>6090000</v>
       </c>
       <c r="MH4" s="4">
-        <v>5599900</v>
+        <v>19556200</v>
       </c>
       <c r="MY4" s="4">
         <v>230530000</v>
@@ -2662,19 +2662,19 @@
         <v>149844500</v>
       </c>
       <c r="NB4" s="4">
-        <v>5530000</v>
+        <v>0</v>
       </c>
       <c r="NC4" s="4">
-        <v>-144314500</v>
+        <v>-149844500</v>
       </c>
       <c r="ND4" s="4">
-        <v>278.86051397091177</v>
+        <v>285.7142857142857</v>
       </c>
       <c r="NE4" s="4">
         <v>0</v>
       </c>
       <c r="NF4" s="4">
-        <v>225000000</v>
+        <v>230530000</v>
       </c>
       <c r="NO4" s="4">
         <v>758120000</v>
@@ -2686,19 +2686,19 @@
         <v>492778000</v>
       </c>
       <c r="NR4" s="4">
-        <v>607420000</v>
+        <v>543580000</v>
       </c>
       <c r="NS4" s="4">
-        <v>114642000</v>
+        <v>50802000</v>
       </c>
       <c r="NT4" s="4">
-        <v>56.794627311168234</v>
+        <v>80.85414295512962</v>
       </c>
       <c r="NU4" s="4">
         <v>77220000</v>
       </c>
       <c r="NV4" s="4">
-        <v>150700000</v>
+        <v>214540000</v>
       </c>
       <c r="PS4" s="4">
         <v>10375000000</v>
@@ -2710,19 +2710,19 @@
         <v>7262500000</v>
       </c>
       <c r="PV4" s="4">
-        <v>7335000000</v>
+        <v>7305000000</v>
       </c>
       <c r="PW4" s="4">
-        <v>72500000</v>
+        <v>42500000</v>
       </c>
       <c r="PX4" s="4">
-        <v>97.6706827309237</v>
+        <v>98.63453815261045</v>
       </c>
       <c r="PY4" s="4">
         <v>2200000000</v>
       </c>
       <c r="PZ4" s="4">
-        <v>3040000000</v>
+        <v>3070000000</v>
       </c>
       <c r="QA4" s="4">
         <v>161739594856</v>
@@ -2734,10 +2734,10 @@
         <v>161739594856</v>
       </c>
       <c r="QD4" s="4">
-        <v>161627295356</v>
+        <v>161212982556</v>
       </c>
       <c r="QE4" s="4">
-        <v>-112299500</v>
+        <v>-526612300</v>
       </c>
       <c r="QF4" s="4">
         <v>0</v>
@@ -2746,7 +2746,7 @@
         <v>59347086558</v>
       </c>
       <c r="QH4" s="4">
-        <v>112299500</v>
+        <v>526612300</v>
       </c>
       <c r="QI4" s="4">
         <v>177242794856</v>
@@ -2758,19 +2758,19 @@
         <v>172055440671</v>
       </c>
       <c r="QL4" s="4">
-        <v>172589538656</v>
+        <v>171966516956</v>
       </c>
       <c r="QM4" s="4">
-        <v>534097985</v>
+        <v>-88923715</v>
       </c>
       <c r="QN4" s="4">
-        <v>-89.70384581518603</v>
+        <v>-101.71424028182105</v>
       </c>
       <c r="QO4" s="4">
         <v>2574678200</v>
       </c>
       <c r="QP4" s="4">
-        <v>-4653256200</v>
+        <v>-5276277900</v>
       </c>
     </row>
     <row r="5">
@@ -6318,19 +6318,19 @@
         <v>40286500</v>
       </c>
       <c r="F11" s="4">
-        <v>51023000</v>
+        <v>60139000</v>
       </c>
       <c r="G11" s="4">
-        <v>10736500</v>
+        <v>19852500</v>
       </c>
       <c r="H11" s="4">
-        <v>73.34963325183375</v>
+        <v>50.721705782334034</v>
       </c>
       <c r="I11" s="4">
         <v>0</v>
       </c>
       <c r="J11" s="4">
-        <v>29550000</v>
+        <v>20434000</v>
       </c>
       <c r="S11" s="4">
         <v>15000000</v>
@@ -6366,19 +6366,19 @@
         <v>11326510</v>
       </c>
       <c r="BB11" s="4">
-        <v>12022500</v>
+        <v>14575200</v>
       </c>
       <c r="BC11" s="4">
-        <v>695990</v>
+        <v>3248690</v>
       </c>
       <c r="BD11" s="4">
-        <v>88.58825130474561</v>
+        <v>46.733094054819816</v>
       </c>
       <c r="BE11" s="4">
         <v>0</v>
       </c>
       <c r="BF11" s="4">
-        <v>5402900</v>
+        <v>2850200</v>
       </c>
       <c r="BG11" s="4">
         <v>2570600</v>
@@ -6390,19 +6390,19 @@
         <v>1670890</v>
       </c>
       <c r="BJ11" s="4">
-        <v>2220900</v>
+        <v>2727700</v>
       </c>
       <c r="BK11" s="4">
-        <v>550010</v>
+        <v>1056810</v>
       </c>
       <c r="BL11" s="4">
-        <v>38.86807971457469</v>
+        <v>-17.46118193640173</v>
       </c>
       <c r="BM11" s="4">
         <v>0</v>
       </c>
       <c r="BN11" s="4">
-        <v>349700</v>
+        <v>-157100</v>
       </c>
       <c r="BO11" s="4">
         <v>521800</v>
@@ -6414,19 +6414,19 @@
         <v>339170</v>
       </c>
       <c r="BR11" s="4">
-        <v>1015600</v>
+        <v>1052200</v>
       </c>
       <c r="BS11" s="4">
-        <v>676430</v>
+        <v>713030</v>
       </c>
       <c r="BT11" s="4">
-        <v>-270.3827410611619</v>
+        <v>-290.42326014345946</v>
       </c>
       <c r="BU11" s="4">
         <v>0</v>
       </c>
       <c r="BV11" s="4">
-        <v>-493800</v>
+        <v>-530400</v>
       </c>
       <c r="CE11" s="4">
         <v>5642000</v>
@@ -6438,19 +6438,19 @@
         <v>3667300</v>
       </c>
       <c r="CH11" s="4">
-        <v>4340000</v>
+        <v>5642000</v>
       </c>
       <c r="CI11" s="4">
-        <v>672700</v>
+        <v>1974700</v>
       </c>
       <c r="CJ11" s="4">
-        <v>65.93406593406594</v>
+        <v>0</v>
       </c>
       <c r="CK11" s="4">
         <v>0</v>
       </c>
       <c r="CL11" s="4">
-        <v>1302000</v>
+        <v>0</v>
       </c>
       <c r="DK11" s="4">
         <v>39140000</v>
@@ -6462,19 +6462,19 @@
         <v>25441000</v>
       </c>
       <c r="DN11" s="4">
-        <v>39140000</v>
+        <v>25441000</v>
       </c>
       <c r="DO11" s="4">
-        <v>13699000</v>
+        <v>0</v>
       </c>
       <c r="DP11" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="DQ11" s="4">
         <v>11305000</v>
       </c>
       <c r="DR11" s="4">
-        <v>0</v>
+        <v>13699000</v>
       </c>
       <c r="EQ11" s="4">
         <v>20622100</v>
@@ -6510,10 +6510,10 @@
         <v>14866094104</v>
       </c>
       <c r="FB11" s="4">
-        <v>14866094104</v>
+        <v>16866094104</v>
       </c>
       <c r="FC11" s="4">
-        <v>0</v>
+        <v>2000000000</v>
       </c>
       <c r="FD11" s="4">
         <v>0</v>
@@ -6522,7 +6522,7 @@
         <v>905893242</v>
       </c>
       <c r="FF11" s="4">
-        <v>0</v>
+        <v>-2000000000</v>
       </c>
       <c r="FG11" s="4">
         <v>15047589004</v>
@@ -6534,19 +6534,19 @@
         <v>14962512104</v>
       </c>
       <c r="FJ11" s="4">
-        <v>14996629104</v>
+        <v>16996444204</v>
       </c>
       <c r="FK11" s="4">
-        <v>34117000</v>
+        <v>2033932100</v>
       </c>
       <c r="FL11" s="4">
-        <v>59.89863288389681</v>
+        <v>-2290.6984151984852</v>
       </c>
       <c r="FM11" s="4">
         <v>11305000</v>
       </c>
       <c r="FN11" s="4">
-        <v>50959900</v>
+        <v>-1948855200</v>
       </c>
       <c r="FO11" s="4">
         <v>247271000</v>
@@ -6558,19 +6558,19 @@
         <v>123635500</v>
       </c>
       <c r="FR11" s="4">
-        <v>72500000</v>
+        <v>65560000</v>
       </c>
       <c r="FS11" s="4">
-        <v>-51135500</v>
+        <v>-58075500</v>
       </c>
       <c r="FT11" s="4">
-        <v>141.35988449919319</v>
+        <v>146.97315900368423</v>
       </c>
       <c r="FU11" s="4">
         <v>0</v>
       </c>
       <c r="FV11" s="4">
-        <v>174771000</v>
+        <v>181711000</v>
       </c>
       <c r="GE11" s="4">
         <v>261550000</v>
@@ -6582,19 +6582,19 @@
         <v>130775000</v>
       </c>
       <c r="GH11" s="4">
-        <v>203500000</v>
+        <v>170250000</v>
       </c>
       <c r="GI11" s="4">
-        <v>72725000</v>
+        <v>39475000</v>
       </c>
       <c r="GJ11" s="4">
-        <v>44.38921812272988</v>
+        <v>69.81456700439686</v>
       </c>
       <c r="GK11" s="4">
         <v>0</v>
       </c>
       <c r="GL11" s="4">
-        <v>58050000</v>
+        <v>91300000</v>
       </c>
       <c r="HK11" s="4">
         <v>21259500</v>
@@ -6726,19 +6726,19 @@
         <v>527906065</v>
       </c>
       <c r="JR11" s="4">
-        <v>534163100</v>
+        <v>493973100</v>
       </c>
       <c r="JS11" s="4">
-        <v>6257035</v>
+        <v>-33932965</v>
       </c>
       <c r="JT11" s="4">
-        <v>97.70041364575069</v>
+        <v>112.47104791218518</v>
       </c>
       <c r="JU11" s="4">
         <v>0</v>
       </c>
       <c r="JV11" s="4">
-        <v>265836900</v>
+        <v>306026900</v>
       </c>
       <c r="JW11" s="4">
         <v>327844000</v>
@@ -6750,19 +6750,19 @@
         <v>163922000</v>
       </c>
       <c r="JZ11" s="4">
-        <v>123523000</v>
+        <v>125699000</v>
       </c>
       <c r="KA11" s="4">
-        <v>-40399000</v>
+        <v>-38223000</v>
       </c>
       <c r="KB11" s="4">
-        <v>124.64525811056477</v>
+        <v>123.31779748904967</v>
       </c>
       <c r="KC11" s="4">
         <v>0</v>
       </c>
       <c r="KD11" s="4">
-        <v>204321000</v>
+        <v>202145000</v>
       </c>
       <c r="KM11" s="4">
         <v>276550000</v>
@@ -6774,19 +6774,19 @@
         <v>138275000</v>
       </c>
       <c r="KP11" s="4">
-        <v>211000000</v>
+        <v>177750000</v>
       </c>
       <c r="KQ11" s="4">
-        <v>72725000</v>
+        <v>39475000</v>
       </c>
       <c r="KR11" s="4">
-        <v>47.40553245344422</v>
+        <v>71.45181703127825</v>
       </c>
       <c r="KS11" s="4">
         <v>0</v>
       </c>
       <c r="KT11" s="4">
-        <v>65550000</v>
+        <v>98800000</v>
       </c>
       <c r="LS11" s="4">
         <v>38684900</v>
@@ -6798,19 +6798,19 @@
         <v>25145185</v>
       </c>
       <c r="LV11" s="4">
-        <v>19764200</v>
+        <v>22316900</v>
       </c>
       <c r="LW11" s="4">
-        <v>-5380985</v>
+        <v>-2828285</v>
       </c>
       <c r="LX11" s="4">
-        <v>139.7422323882002</v>
+        <v>120.88880748228452</v>
       </c>
       <c r="LY11" s="4">
         <v>0</v>
       </c>
       <c r="LZ11" s="4">
-        <v>18920700</v>
+        <v>16368000</v>
       </c>
       <c r="MA11" s="4">
         <v>6307700</v>
@@ -6822,19 +6822,19 @@
         <v>4100005</v>
       </c>
       <c r="MD11" s="4">
-        <v>3239600</v>
+        <v>3746400</v>
       </c>
       <c r="ME11" s="4">
-        <v>-860405</v>
+        <v>-353605</v>
       </c>
       <c r="MF11" s="4">
-        <v>138.9730012524375</v>
+        <v>116.01693168666867</v>
       </c>
       <c r="MG11" s="4">
         <v>0</v>
       </c>
       <c r="MH11" s="4">
-        <v>3068100</v>
+        <v>2561300</v>
       </c>
       <c r="MQ11" s="4">
         <v>11397500</v>
@@ -6870,19 +6870,19 @@
         <v>12851800</v>
       </c>
       <c r="NB11" s="4">
-        <v>12332000</v>
+        <v>13634000</v>
       </c>
       <c r="NC11" s="4">
-        <v>-519800</v>
+        <v>782200</v>
       </c>
       <c r="ND11" s="4">
-        <v>107.51134360278604</v>
+        <v>88.69685847229849</v>
       </c>
       <c r="NE11" s="4">
         <v>0</v>
       </c>
       <c r="NF11" s="4">
-        <v>7440000</v>
+        <v>6138000</v>
       </c>
       <c r="QA11" s="4">
         <v>15102323204</v>
@@ -6894,10 +6894,10 @@
         <v>15102323204</v>
       </c>
       <c r="QD11" s="4">
-        <v>15102323204</v>
+        <v>17102323204</v>
       </c>
       <c r="QE11" s="4">
-        <v>0</v>
+        <v>2000000000</v>
       </c>
       <c r="QF11" s="4">
         <v>0</v>
@@ -6906,7 +6906,7 @@
         <v>905893242</v>
       </c>
       <c r="QH11" s="4">
-        <v>0</v>
+        <v>-2000000000</v>
       </c>
       <c r="QI11" s="4">
         <v>15847589004</v>
@@ -6918,19 +6918,19 @@
         <v>15490418169</v>
       </c>
       <c r="QL11" s="4">
-        <v>15530792204</v>
+        <v>17490417304</v>
       </c>
       <c r="QM11" s="4">
-        <v>40374035</v>
+        <v>1999999135</v>
       </c>
       <c r="QN11" s="4">
-        <v>-88.69615572055316</v>
+        <v>459.95589197533445</v>
       </c>
       <c r="QO11" s="4">
         <v>11305000</v>
       </c>
       <c r="QP11" s="4">
-        <v>-316796800</v>
+        <v>1642828300</v>
       </c>
     </row>
     <row r="12">
@@ -9702,19 +9702,19 @@
         <v>19139445</v>
       </c>
       <c r="BB17" s="4">
-        <v>19521600</v>
+        <v>21519600</v>
       </c>
       <c r="BC17" s="4">
-        <v>382155</v>
+        <v>2380155</v>
       </c>
       <c r="BD17" s="4">
-        <v>96.29186515820376</v>
+        <v>76.90482740151108</v>
       </c>
       <c r="BE17" s="4">
         <v>4310500</v>
       </c>
       <c r="BF17" s="4">
-        <v>9923700</v>
+        <v>7925700</v>
       </c>
       <c r="BG17" s="4">
         <v>8298100</v>
@@ -9726,19 +9726,19 @@
         <v>5393765</v>
       </c>
       <c r="BJ17" s="4">
-        <v>5696200</v>
+        <v>11873200</v>
       </c>
       <c r="BK17" s="4">
-        <v>302435</v>
+        <v>6479435</v>
       </c>
       <c r="BL17" s="4">
-        <v>89.58677287571854</v>
+        <v>-123.0953040885435</v>
       </c>
       <c r="BM17" s="4">
         <v>1832500</v>
       </c>
       <c r="BN17" s="4">
-        <v>2601900</v>
+        <v>-3575100</v>
       </c>
       <c r="BO17" s="4">
         <v>20324700</v>
@@ -9822,10 +9822,10 @@
         <v>2512304931</v>
       </c>
       <c r="FB17" s="4">
-        <v>2512304931</v>
+        <v>2593592931</v>
       </c>
       <c r="FC17" s="4">
-        <v>0</v>
+        <v>81288000</v>
       </c>
       <c r="FD17" s="4">
         <v>0</v>
@@ -9834,7 +9834,7 @@
         <v>970827019</v>
       </c>
       <c r="FF17" s="4">
-        <v>0</v>
+        <v>-81288000</v>
       </c>
       <c r="FG17" s="4">
         <v>2714829031</v>
@@ -9846,19 +9846,19 @@
         <v>2628520196</v>
       </c>
       <c r="FJ17" s="4">
-        <v>2629043131</v>
+        <v>2718506131</v>
       </c>
       <c r="FK17" s="4">
-        <v>522935</v>
+        <v>89985935</v>
       </c>
       <c r="FL17" s="4">
-        <v>99.39411185424991</v>
+        <v>-4.260398138846388</v>
       </c>
       <c r="FM17" s="4">
         <v>41791100</v>
       </c>
       <c r="FN17" s="4">
-        <v>85785900</v>
+        <v>-3677100</v>
       </c>
       <c r="FO17" s="4">
         <v>261131000</v>
@@ -10062,19 +10062,19 @@
         <v>25798110</v>
       </c>
       <c r="LV17" s="4">
-        <v>30371200</v>
+        <v>32369200</v>
       </c>
       <c r="LW17" s="4">
-        <v>4573090</v>
+        <v>6571090</v>
       </c>
       <c r="LX17" s="4">
-        <v>67.0794433058413</v>
+        <v>52.69632985849406</v>
       </c>
       <c r="LY17" s="4">
         <v>4310500</v>
       </c>
       <c r="LZ17" s="4">
-        <v>9318200</v>
+        <v>7320200</v>
       </c>
       <c r="MA17" s="4">
         <v>8298100</v>
@@ -10086,19 +10086,19 @@
         <v>5393765</v>
       </c>
       <c r="MD17" s="4">
-        <v>5696200</v>
+        <v>11873200</v>
       </c>
       <c r="ME17" s="4">
-        <v>302435</v>
+        <v>6479435</v>
       </c>
       <c r="MF17" s="4">
-        <v>89.58677287571854</v>
+        <v>-123.0953040885435</v>
       </c>
       <c r="MG17" s="4">
         <v>1832500</v>
       </c>
       <c r="MH17" s="4">
-        <v>2601900</v>
+        <v>-3575100</v>
       </c>
       <c r="MY17" s="4">
         <v>52525000</v>
@@ -10134,10 +10134,10 @@
         <v>2526304931</v>
       </c>
       <c r="QD17" s="4">
-        <v>2526304931</v>
+        <v>2607592931</v>
       </c>
       <c r="QE17" s="4">
-        <v>0</v>
+        <v>81288000</v>
       </c>
       <c r="QF17" s="4">
         <v>0</v>
@@ -10146,7 +10146,7 @@
         <v>970827019</v>
       </c>
       <c r="QH17" s="4">
-        <v>0</v>
+        <v>-81288000</v>
       </c>
       <c r="QI17" s="4">
         <v>3214828931</v>
@@ -10158,19 +10158,19 @@
         <v>2896165911</v>
       </c>
       <c r="QL17" s="4">
-        <v>2896688331</v>
+        <v>2986151331</v>
       </c>
       <c r="QM17" s="4">
-        <v>522420</v>
+        <v>89985420</v>
       </c>
       <c r="QN17" s="4">
-        <v>-99.83605879339247</v>
+        <v>-71.7615743427022</v>
       </c>
       <c r="QO17" s="4">
         <v>41791100</v>
       </c>
       <c r="QP17" s="4">
-        <v>-318140600</v>
+        <v>-228677600</v>
       </c>
     </row>
     <row r="18">
@@ -10238,19 +10238,19 @@
         <v>18185050</v>
       </c>
       <c r="BB18" s="4">
-        <v>22174300</v>
+        <v>21789900</v>
       </c>
       <c r="BC18" s="4">
-        <v>3989250</v>
+        <v>3604850</v>
       </c>
       <c r="BD18" s="4">
-        <v>59.25990226665782</v>
+        <v>63.18557590673972</v>
       </c>
       <c r="BE18" s="4">
         <v>21387000</v>
       </c>
       <c r="BF18" s="4">
-        <v>5802700</v>
+        <v>6187100</v>
       </c>
       <c r="BG18" s="4">
         <v>5279400</v>
@@ -10358,19 +10358,19 @@
         <v>4066179187</v>
       </c>
       <c r="FJ18" s="4">
-        <v>4113423007</v>
+        <v>4113038607</v>
       </c>
       <c r="FK18" s="4">
-        <v>47243820</v>
+        <v>46859420</v>
       </c>
       <c r="FL18" s="4">
-        <v>51.23883997456038</v>
+        <v>51.6355858328288</v>
       </c>
       <c r="FM18" s="4">
         <v>110978460</v>
       </c>
       <c r="FN18" s="4">
-        <v>49644400</v>
+        <v>50028800</v>
       </c>
       <c r="GE18" s="4">
         <v>259700000</v>
@@ -10382,19 +10382,19 @@
         <v>129850000</v>
       </c>
       <c r="GH18" s="4">
-        <v>93750000</v>
+        <v>87350000</v>
       </c>
       <c r="GI18" s="4">
-        <v>-36100000</v>
+        <v>-42500000</v>
       </c>
       <c r="GJ18" s="4">
-        <v>127.80130920292645</v>
+        <v>132.73007316134</v>
       </c>
       <c r="GK18" s="4">
         <v>3500000</v>
       </c>
       <c r="GL18" s="4">
-        <v>165950000</v>
+        <v>172350000</v>
       </c>
       <c r="GU18" s="4">
         <v>413859000</v>
@@ -10406,19 +10406,19 @@
         <v>206929500</v>
       </c>
       <c r="GX18" s="4">
-        <v>284013000</v>
+        <v>290489000</v>
       </c>
       <c r="GY18" s="4">
-        <v>77083500</v>
+        <v>83559500</v>
       </c>
       <c r="GZ18" s="4">
-        <v>62.74890723652259</v>
+        <v>59.619338953604974</v>
       </c>
       <c r="HA18" s="4">
         <v>65556260</v>
       </c>
       <c r="HB18" s="4">
-        <v>129846000</v>
+        <v>123370000</v>
       </c>
       <c r="HK18" s="4">
         <v>14896000</v>
@@ -10430,19 +10430,19 @@
         <v>9682400</v>
       </c>
       <c r="HN18" s="4">
-        <v>8582600</v>
+        <v>8967000</v>
       </c>
       <c r="HO18" s="4">
-        <v>-1099800</v>
+        <v>-715400</v>
       </c>
       <c r="HP18" s="4">
-        <v>121.0948289090072</v>
+        <v>113.72180451127821</v>
       </c>
       <c r="HQ18" s="4">
         <v>21387000</v>
       </c>
       <c r="HR18" s="4">
-        <v>6313400</v>
+        <v>5929000</v>
       </c>
       <c r="HS18" s="4">
         <v>2498700</v>
@@ -10502,10 +10502,10 @@
         <v>50661600</v>
       </c>
       <c r="JJ18" s="4">
-        <v>25403000</v>
+        <v>25327400</v>
       </c>
       <c r="JK18" s="4">
-        <v>-25258600</v>
+        <v>-25334200</v>
       </c>
       <c r="JL18" s="4">
         <v>0</v>
@@ -10514,7 +10514,7 @@
         <v>13241200</v>
       </c>
       <c r="JN18" s="4">
-        <v>25258600</v>
+        <v>25334200</v>
       </c>
       <c r="JO18" s="4">
         <v>899615300</v>
@@ -10526,19 +10526,19 @@
         <v>501447655</v>
       </c>
       <c r="JR18" s="4">
-        <v>453747300</v>
+        <v>454132100</v>
       </c>
       <c r="JS18" s="4">
-        <v>-47700355</v>
+        <v>-47315555</v>
       </c>
       <c r="JT18" s="4">
-        <v>111.97996763398493</v>
+        <v>111.88332492460556</v>
       </c>
       <c r="JU18" s="4">
         <v>99206060</v>
       </c>
       <c r="JV18" s="4">
-        <v>445868000</v>
+        <v>445483200</v>
       </c>
       <c r="KM18" s="4">
         <v>305400000</v>
@@ -10550,19 +10550,19 @@
         <v>152700000</v>
       </c>
       <c r="KP18" s="4">
-        <v>127100000</v>
+        <v>120700000</v>
       </c>
       <c r="KQ18" s="4">
-        <v>-25600000</v>
+        <v>-32000000</v>
       </c>
       <c r="KR18" s="4">
-        <v>116.76489849377865</v>
+        <v>120.95612311722333</v>
       </c>
       <c r="KS18" s="4">
         <v>3500000</v>
       </c>
       <c r="KT18" s="4">
-        <v>178300000</v>
+        <v>184700000</v>
       </c>
       <c r="LC18" s="4">
         <v>499839000</v>
@@ -10574,19 +10574,19 @@
         <v>249919500</v>
       </c>
       <c r="LF18" s="4">
-        <v>346629000</v>
+        <v>353105000</v>
       </c>
       <c r="LG18" s="4">
-        <v>96709500</v>
+        <v>103185500</v>
       </c>
       <c r="LH18" s="4">
-        <v>61.30373980421696</v>
+        <v>58.712505426747406</v>
       </c>
       <c r="LI18" s="4">
         <v>65556260</v>
       </c>
       <c r="LJ18" s="4">
-        <v>153210000</v>
+        <v>146734000</v>
       </c>
       <c r="LS18" s="4">
         <v>42873000</v>
@@ -10694,19 +10694,19 @@
         <v>4567626842</v>
       </c>
       <c r="QL18" s="4">
-        <v>4567170307</v>
+        <v>4567170707</v>
       </c>
       <c r="QM18" s="4">
-        <v>-456535</v>
+        <v>-456135</v>
       </c>
       <c r="QN18" s="4">
-        <v>-100.09221888523632</v>
+        <v>-100.09213808627437</v>
       </c>
       <c r="QO18" s="4">
         <v>110978460</v>
       </c>
       <c r="QP18" s="4">
-        <v>-495512400</v>
+        <v>-495512000</v>
       </c>
     </row>
     <row r="19">
@@ -10822,19 +10822,19 @@
         <v>8378045</v>
       </c>
       <c r="BR19" s="4">
-        <v>10400700</v>
+        <v>9803100</v>
       </c>
       <c r="BS19" s="4">
-        <v>2022655</v>
+        <v>1425055</v>
       </c>
       <c r="BT19" s="4">
-        <v>55.164250302853645</v>
+        <v>68.41111841383385</v>
       </c>
       <c r="BU19" s="4">
         <v>6026400</v>
       </c>
       <c r="BV19" s="4">
-        <v>2488600</v>
+        <v>3086200</v>
       </c>
       <c r="CE19" s="4">
         <v>10912000</v>
@@ -10918,10 +10918,10 @@
         <v>1725859450</v>
       </c>
       <c r="FB19" s="4">
-        <v>1714281050</v>
+        <v>1707401050</v>
       </c>
       <c r="FC19" s="4">
-        <v>-11578400</v>
+        <v>-18458400</v>
       </c>
       <c r="FD19" s="4">
         <v>0</v>
@@ -10930,7 +10930,7 @@
         <v>549797477</v>
       </c>
       <c r="FF19" s="4">
-        <v>11578400</v>
+        <v>18458400</v>
       </c>
       <c r="FG19" s="4">
         <v>2000281850</v>
@@ -10942,19 +10942,19 @@
         <v>1881255930</v>
       </c>
       <c r="FJ19" s="4">
-        <v>1888921610</v>
+        <v>1881444010</v>
       </c>
       <c r="FK19" s="4">
-        <v>7665680</v>
+        <v>188080</v>
       </c>
       <c r="FL19" s="4">
-        <v>93.55965490541892</v>
+        <v>99.8419839981073</v>
       </c>
       <c r="FM19" s="4">
         <v>239110335</v>
       </c>
       <c r="FN19" s="4">
-        <v>111360240</v>
+        <v>118837840</v>
       </c>
       <c r="JW19" s="4">
         <v>84787200</v>
@@ -11086,10 +11086,10 @@
         <v>1725859450</v>
       </c>
       <c r="QD19" s="4">
-        <v>1714281050</v>
+        <v>1707401050</v>
       </c>
       <c r="QE19" s="4">
-        <v>-11578400</v>
+        <v>-18458400</v>
       </c>
       <c r="QF19" s="4">
         <v>0</v>
@@ -11098,7 +11098,7 @@
         <v>549797477</v>
       </c>
       <c r="QH19" s="4">
-        <v>11578400</v>
+        <v>18458400</v>
       </c>
       <c r="QI19" s="4">
         <v>2000281850</v>
@@ -11110,19 +11110,19 @@
         <v>1881255930</v>
       </c>
       <c r="QL19" s="4">
-        <v>1888921610</v>
+        <v>1881444010</v>
       </c>
       <c r="QM19" s="4">
-        <v>7665680</v>
+        <v>188080</v>
       </c>
       <c r="QN19" s="4">
-        <v>-93.55965490541892</v>
+        <v>-99.8419839981073</v>
       </c>
       <c r="QO19" s="4">
         <v>239110335</v>
       </c>
       <c r="QP19" s="4">
-        <v>-111360240</v>
+        <v>-118837840</v>
       </c>
     </row>
     <row r="20">
@@ -14278,10 +14278,10 @@
         <v>1750844300</v>
       </c>
       <c r="JJ25" s="4">
-        <v>1666235900</v>
+        <v>1716235900</v>
       </c>
       <c r="JK25" s="4">
-        <v>-84608400</v>
+        <v>-34608400</v>
       </c>
       <c r="JL25" s="4">
         <v>0</v>
@@ -14290,7 +14290,7 @@
         <v>17467600</v>
       </c>
       <c r="JN25" s="4">
-        <v>84608400</v>
+        <v>34608400</v>
       </c>
       <c r="JO25" s="4">
         <v>2650000100</v>
@@ -14302,19 +14302,19 @@
         <v>2266440620</v>
       </c>
       <c r="JR25" s="4">
-        <v>2197819500</v>
+        <v>2247819500</v>
       </c>
       <c r="JS25" s="4">
-        <v>-68621120</v>
+        <v>-18621120</v>
       </c>
       <c r="JT25" s="4">
-        <v>117.89060721429698</v>
+        <v>104.85481938811681</v>
       </c>
       <c r="JU25" s="4">
         <v>105267860</v>
       </c>
       <c r="JV25" s="4">
-        <v>452180600</v>
+        <v>402180600</v>
       </c>
       <c r="JW25" s="4">
         <v>286093000</v>
@@ -14494,10 +14494,10 @@
         <v>4194079694</v>
       </c>
       <c r="QD25" s="4">
-        <v>4118076394</v>
+        <v>4168076394</v>
       </c>
       <c r="QE25" s="4">
-        <v>-76003300</v>
+        <v>-26003300</v>
       </c>
       <c r="QF25" s="4">
         <v>0</v>
@@ -14506,7 +14506,7 @@
         <v>924120101</v>
       </c>
       <c r="QH25" s="4">
-        <v>76003300</v>
+        <v>26003300</v>
       </c>
       <c r="QI25" s="4">
         <v>5367175694</v>
@@ -14518,19 +14518,19 @@
         <v>4904834619</v>
       </c>
       <c r="QL25" s="4">
-        <v>4825845694</v>
+        <v>4875845694</v>
       </c>
       <c r="QM25" s="4">
-        <v>-78988925</v>
+        <v>-28988925</v>
       </c>
       <c r="QN25" s="4">
-        <v>-117.0845571097052</v>
+        <v>-106.27003019361842</v>
       </c>
       <c r="QO25" s="4">
         <v>115346460</v>
       </c>
       <c r="QP25" s="4">
-        <v>-541330000</v>
+        <v>-491330000</v>
       </c>
     </row>
     <row r="26">
@@ -16742,19 +16742,19 @@
         <v>56837500</v>
       </c>
       <c r="V30" s="4">
-        <v>64675000</v>
+        <v>86325000</v>
       </c>
       <c r="W30" s="4">
-        <v>7837500</v>
+        <v>29487500</v>
       </c>
       <c r="X30" s="4">
-        <v>86.21068836595558</v>
+        <v>48.119639322630306</v>
       </c>
       <c r="Y30" s="4">
         <v>37525000</v>
       </c>
       <c r="Z30" s="4">
-        <v>49000000</v>
+        <v>27350000</v>
       </c>
       <c r="AI30" s="4">
         <v>499826000</v>
@@ -16766,19 +16766,19 @@
         <v>249913000</v>
       </c>
       <c r="AL30" s="4">
-        <v>268548000</v>
+        <v>291003000</v>
       </c>
       <c r="AM30" s="4">
-        <v>18635000</v>
+        <v>41090000</v>
       </c>
       <c r="AN30" s="4">
-        <v>92.54340510497653</v>
+        <v>83.55827828084173</v>
       </c>
       <c r="AO30" s="4">
         <v>17031600</v>
       </c>
       <c r="AP30" s="4">
-        <v>231278000</v>
+        <v>208823000</v>
       </c>
       <c r="AY30" s="4">
         <v>13159000</v>
@@ -16790,19 +16790,19 @@
         <v>8553350</v>
       </c>
       <c r="BB30" s="4">
-        <v>7981900</v>
+        <v>10342300</v>
       </c>
       <c r="BC30" s="4">
-        <v>-571450</v>
+        <v>1788950</v>
       </c>
       <c r="BD30" s="4">
-        <v>112.40758633417649</v>
+        <v>61.157491342155836</v>
       </c>
       <c r="BE30" s="4">
         <v>3785800</v>
       </c>
       <c r="BF30" s="4">
-        <v>5177100</v>
+        <v>2816700</v>
       </c>
       <c r="BG30" s="4">
         <v>17490500</v>
@@ -16814,19 +16814,19 @@
         <v>11368825</v>
       </c>
       <c r="BJ30" s="4">
-        <v>5189500</v>
+        <v>6490100</v>
       </c>
       <c r="BK30" s="4">
-        <v>-6179325</v>
+        <v>-4878725</v>
       </c>
       <c r="BL30" s="4">
-        <v>200.94173571775698</v>
+        <v>179.69591655878497</v>
       </c>
       <c r="BM30" s="4">
         <v>1966700</v>
       </c>
       <c r="BN30" s="4">
-        <v>12301000</v>
+        <v>11000400</v>
       </c>
       <c r="BO30" s="4">
         <v>74841500</v>
@@ -16838,19 +16838,19 @@
         <v>48646975</v>
       </c>
       <c r="BR30" s="4">
-        <v>38049600</v>
+        <v>38766600</v>
       </c>
       <c r="BS30" s="4">
-        <v>-10597375</v>
+        <v>-9880375</v>
       </c>
       <c r="BT30" s="4">
-        <v>140.45645034601696</v>
+        <v>137.71923713065993</v>
       </c>
       <c r="BU30" s="4">
         <v>3240600</v>
       </c>
       <c r="BV30" s="4">
-        <v>36791900</v>
+        <v>36074900</v>
       </c>
       <c r="CE30" s="4">
         <v>26970000</v>
@@ -16862,19 +16862,19 @@
         <v>17530500</v>
       </c>
       <c r="CH30" s="4">
-        <v>20506000</v>
+        <v>21856000</v>
       </c>
       <c r="CI30" s="4">
-        <v>2975500</v>
+        <v>4325500</v>
       </c>
       <c r="CJ30" s="4">
-        <v>68.47820329466603</v>
+        <v>54.176598336776316</v>
       </c>
       <c r="CK30" s="4">
         <v>1922000</v>
       </c>
       <c r="CL30" s="4">
-        <v>6464000</v>
+        <v>5114000</v>
       </c>
       <c r="EY30" s="4">
         <v>48301000</v>
@@ -16886,10 +16886,10 @@
         <v>48301000</v>
       </c>
       <c r="FB30" s="4">
-        <v>36201000</v>
+        <v>36368000</v>
       </c>
       <c r="FC30" s="4">
-        <v>-12100000</v>
+        <v>-11933000</v>
       </c>
       <c r="FD30" s="4">
         <v>0</v>
@@ -16898,7 +16898,7 @@
         <v>1336000</v>
       </c>
       <c r="FF30" s="4">
-        <v>12100000</v>
+        <v>11933000</v>
       </c>
       <c r="FG30" s="4">
         <v>794263000</v>
@@ -16910,19 +16910,19 @@
         <v>441151150</v>
       </c>
       <c r="FJ30" s="4">
-        <v>441151000</v>
+        <v>491151000</v>
       </c>
       <c r="FK30" s="4">
-        <v>-150</v>
+        <v>49999850</v>
       </c>
       <c r="FL30" s="4">
-        <v>100.00004247945799</v>
+        <v>85.84022314742482</v>
       </c>
       <c r="FM30" s="4">
         <v>65471700</v>
       </c>
       <c r="FN30" s="4">
-        <v>353112000</v>
+        <v>303112000</v>
       </c>
       <c r="KM30" s="4">
         <v>113675000</v>
@@ -16934,19 +16934,19 @@
         <v>56837500</v>
       </c>
       <c r="KP30" s="4">
-        <v>64675000</v>
+        <v>86325000</v>
       </c>
       <c r="KQ30" s="4">
-        <v>7837500</v>
+        <v>29487500</v>
       </c>
       <c r="KR30" s="4">
-        <v>86.21068836595558</v>
+        <v>48.119639322630306</v>
       </c>
       <c r="KS30" s="4">
         <v>37525000</v>
       </c>
       <c r="KT30" s="4">
-        <v>49000000</v>
+        <v>27350000</v>
       </c>
       <c r="LC30" s="4">
         <v>499826000</v>
@@ -16958,19 +16958,19 @@
         <v>249913000</v>
       </c>
       <c r="LF30" s="4">
-        <v>268548000</v>
+        <v>291003000</v>
       </c>
       <c r="LG30" s="4">
-        <v>18635000</v>
+        <v>41090000</v>
       </c>
       <c r="LH30" s="4">
-        <v>92.54340510497653</v>
+        <v>83.55827828084173</v>
       </c>
       <c r="LI30" s="4">
         <v>17031600</v>
       </c>
       <c r="LJ30" s="4">
-        <v>231278000</v>
+        <v>208823000</v>
       </c>
       <c r="LS30" s="4">
         <v>13159000</v>
@@ -16982,19 +16982,19 @@
         <v>8553350</v>
       </c>
       <c r="LV30" s="4">
-        <v>7981900</v>
+        <v>10342300</v>
       </c>
       <c r="LW30" s="4">
-        <v>-571450</v>
+        <v>1788950</v>
       </c>
       <c r="LX30" s="4">
-        <v>112.40758633417649</v>
+        <v>61.157491342155836</v>
       </c>
       <c r="LY30" s="4">
         <v>3785800</v>
       </c>
       <c r="LZ30" s="4">
-        <v>5177100</v>
+        <v>2816700</v>
       </c>
       <c r="MA30" s="4">
         <v>17490500</v>
@@ -17006,19 +17006,19 @@
         <v>11368825</v>
       </c>
       <c r="MD30" s="4">
-        <v>5189500</v>
+        <v>6490100</v>
       </c>
       <c r="ME30" s="4">
-        <v>-6179325</v>
+        <v>-4878725</v>
       </c>
       <c r="MF30" s="4">
-        <v>200.94173571775698</v>
+        <v>179.69591655878497</v>
       </c>
       <c r="MG30" s="4">
         <v>1966700</v>
       </c>
       <c r="MH30" s="4">
-        <v>12301000</v>
+        <v>11000400</v>
       </c>
       <c r="MY30" s="4">
         <v>26970000</v>
@@ -17030,19 +17030,19 @@
         <v>17530500</v>
       </c>
       <c r="NB30" s="4">
-        <v>20506000</v>
+        <v>21856000</v>
       </c>
       <c r="NC30" s="4">
-        <v>2975500</v>
+        <v>4325500</v>
       </c>
       <c r="ND30" s="4">
-        <v>68.47820329466603</v>
+        <v>54.176598336776316</v>
       </c>
       <c r="NE30" s="4">
         <v>1922000</v>
       </c>
       <c r="NF30" s="4">
-        <v>6464000</v>
+        <v>5114000</v>
       </c>
       <c r="QA30" s="4">
         <v>48301000</v>
@@ -17054,10 +17054,10 @@
         <v>48301000</v>
       </c>
       <c r="QD30" s="4">
-        <v>36201000</v>
+        <v>36368000</v>
       </c>
       <c r="QE30" s="4">
-        <v>-12100000</v>
+        <v>-11933000</v>
       </c>
       <c r="QF30" s="4">
         <v>0</v>
@@ -17066,7 +17066,7 @@
         <v>1336000</v>
       </c>
       <c r="QH30" s="4">
-        <v>12100000</v>
+        <v>11933000</v>
       </c>
       <c r="QI30" s="4">
         <v>794263000</v>
@@ -17078,19 +17078,19 @@
         <v>441151150</v>
       </c>
       <c r="QL30" s="4">
-        <v>441151000</v>
+        <v>491151000</v>
       </c>
       <c r="QM30" s="4">
-        <v>-150</v>
+        <v>49999850</v>
       </c>
       <c r="QN30" s="4">
-        <v>-100.00004247945799</v>
+        <v>-85.84022314742482</v>
       </c>
       <c r="QO30" s="4">
         <v>65471700</v>
       </c>
       <c r="QP30" s="4">
-        <v>-353112000</v>
+        <v>-303112000</v>
       </c>
     </row>
     <row r="31">
@@ -17966,19 +17966,19 @@
         <v>126684000</v>
       </c>
       <c r="F33" s="4">
-        <v>139888000</v>
+        <v>135836000</v>
       </c>
       <c r="G33" s="4">
-        <v>13204000</v>
+        <v>9152000</v>
       </c>
       <c r="H33" s="4">
-        <v>89.57721574942377</v>
+        <v>92.77572542704682</v>
       </c>
       <c r="I33" s="4">
         <v>25820000</v>
       </c>
       <c r="J33" s="4">
-        <v>113480000</v>
+        <v>117532000</v>
       </c>
       <c r="AI33" s="4">
         <v>257234000</v>
@@ -18014,19 +18014,19 @@
         <v>18071365</v>
       </c>
       <c r="BB33" s="4">
-        <v>18660300</v>
+        <v>20478900</v>
       </c>
       <c r="BC33" s="4">
-        <v>588935</v>
+        <v>2407535</v>
       </c>
       <c r="BD33" s="4">
-        <v>93.94768226655027</v>
+        <v>75.25844656133376</v>
       </c>
       <c r="BE33" s="4">
         <v>19176700</v>
       </c>
       <c r="BF33" s="4">
-        <v>9141800</v>
+        <v>7323200</v>
       </c>
       <c r="BG33" s="4">
         <v>14060600</v>
@@ -18062,19 +18062,19 @@
         <v>9458280</v>
       </c>
       <c r="BR33" s="4">
-        <v>11113800</v>
+        <v>11403000</v>
       </c>
       <c r="BS33" s="4">
-        <v>1655520</v>
+        <v>1944720</v>
       </c>
       <c r="BT33" s="4">
-        <v>67.4936971324898</v>
+        <v>61.81522584293489</v>
       </c>
       <c r="BU33" s="4">
         <v>1767676</v>
       </c>
       <c r="BV33" s="4">
-        <v>3437400</v>
+        <v>3148200</v>
       </c>
       <c r="CE33" s="4">
         <v>25799000</v>
@@ -18086,19 +18086,19 @@
         <v>16769350</v>
       </c>
       <c r="CH33" s="4">
-        <v>18675000</v>
+        <v>20574000</v>
       </c>
       <c r="CI33" s="4">
-        <v>1905650</v>
+        <v>3804650</v>
       </c>
       <c r="CJ33" s="4">
-        <v>78.89563825840426</v>
+        <v>57.86492278216764</v>
       </c>
       <c r="CK33" s="4">
         <v>0</v>
       </c>
       <c r="CL33" s="4">
-        <v>7124000</v>
+        <v>5225000</v>
       </c>
       <c r="EY33" s="4">
         <v>64817900</v>
@@ -18134,19 +18134,19 @@
         <v>373557285</v>
       </c>
       <c r="FJ33" s="4">
-        <v>372928100</v>
+        <v>372882900</v>
       </c>
       <c r="FK33" s="4">
-        <v>-629185</v>
+        <v>-674385</v>
       </c>
       <c r="FL33" s="4">
-        <v>100.22148512165859</v>
+        <v>100.23739638384532</v>
       </c>
       <c r="FM33" s="4">
         <v>98324560</v>
       </c>
       <c r="FN33" s="4">
-        <v>284704700</v>
+        <v>284749900</v>
       </c>
       <c r="JW33" s="4">
         <v>253368000</v>
@@ -18158,19 +18158,19 @@
         <v>126684000</v>
       </c>
       <c r="JZ33" s="4">
-        <v>139888000</v>
+        <v>135836000</v>
       </c>
       <c r="KA33" s="4">
-        <v>13204000</v>
+        <v>9152000</v>
       </c>
       <c r="KB33" s="4">
-        <v>89.57721574942377</v>
+        <v>92.77572542704682</v>
       </c>
       <c r="KC33" s="4">
         <v>25820000</v>
       </c>
       <c r="KD33" s="4">
-        <v>113480000</v>
+        <v>117532000</v>
       </c>
       <c r="LC33" s="4">
         <v>257234000</v>
@@ -18206,19 +18206,19 @@
         <v>18071365</v>
       </c>
       <c r="LV33" s="4">
-        <v>18660300</v>
+        <v>20478900</v>
       </c>
       <c r="LW33" s="4">
-        <v>588935</v>
+        <v>2407535</v>
       </c>
       <c r="LX33" s="4">
-        <v>93.94768226655027</v>
+        <v>75.25844656133376</v>
       </c>
       <c r="LY33" s="4">
         <v>19176700</v>
       </c>
       <c r="LZ33" s="4">
-        <v>9141800</v>
+        <v>7323200</v>
       </c>
       <c r="MA33" s="4">
         <v>14060600</v>
@@ -18254,19 +18254,19 @@
         <v>16769350</v>
       </c>
       <c r="NB33" s="4">
-        <v>18675000</v>
+        <v>20574000</v>
       </c>
       <c r="NC33" s="4">
-        <v>1905650</v>
+        <v>3804650</v>
       </c>
       <c r="ND33" s="4">
-        <v>78.89563825840426</v>
+        <v>57.86492278216764</v>
       </c>
       <c r="NE33" s="4">
         <v>0</v>
       </c>
       <c r="NF33" s="4">
-        <v>7124000</v>
+        <v>5225000</v>
       </c>
       <c r="QA33" s="4">
         <v>64817900</v>
@@ -18302,19 +18302,19 @@
         <v>373557285</v>
       </c>
       <c r="QL33" s="4">
-        <v>372928100</v>
+        <v>372882900</v>
       </c>
       <c r="QM33" s="4">
-        <v>-629185</v>
+        <v>-674385</v>
       </c>
       <c r="QN33" s="4">
-        <v>-100.22148512165859</v>
+        <v>-100.23739638384532</v>
       </c>
       <c r="QO33" s="4">
         <v>98324560</v>
       </c>
       <c r="QP33" s="4">
-        <v>-284704700</v>
+        <v>-284749900</v>
       </c>
     </row>
     <row r="34">
@@ -18750,19 +18750,19 @@
         <v>256350500</v>
       </c>
       <c r="F35" s="4">
-        <v>245707000</v>
+        <v>245588000</v>
       </c>
       <c r="G35" s="4">
-        <v>-10643500</v>
+        <v>-10762500</v>
       </c>
       <c r="H35" s="4">
-        <v>104.15193260789425</v>
+        <v>104.198353426266</v>
       </c>
       <c r="I35" s="4">
         <v>147531240</v>
       </c>
       <c r="J35" s="4">
-        <v>266994000</v>
+        <v>267113000</v>
       </c>
       <c r="S35" s="4">
         <v>19000000</v>
@@ -18918,19 +18918,19 @@
         <v>332470915</v>
       </c>
       <c r="FJ35" s="4">
-        <v>332469700</v>
+        <v>332350700</v>
       </c>
       <c r="FK35" s="4">
-        <v>-1215</v>
+        <v>-120215</v>
       </c>
       <c r="FL35" s="4">
-        <v>100.00040903473912</v>
+        <v>100.04047087338527</v>
       </c>
       <c r="FM35" s="4">
         <v>171498140</v>
       </c>
       <c r="FN35" s="4">
-        <v>297042000</v>
+        <v>297161000</v>
       </c>
       <c r="JW35" s="4">
         <v>512701000</v>
@@ -18942,19 +18942,19 @@
         <v>256350500</v>
       </c>
       <c r="JZ35" s="4">
-        <v>245707000</v>
+        <v>245588000</v>
       </c>
       <c r="KA35" s="4">
-        <v>-10643500</v>
+        <v>-10762500</v>
       </c>
       <c r="KB35" s="4">
-        <v>104.15193260789425</v>
+        <v>104.198353426266</v>
       </c>
       <c r="KC35" s="4">
         <v>147531240</v>
       </c>
       <c r="KD35" s="4">
-        <v>266994000</v>
+        <v>267113000</v>
       </c>
       <c r="KM35" s="4">
         <v>19000000</v>
@@ -19086,19 +19086,19 @@
         <v>332470915</v>
       </c>
       <c r="QL35" s="4">
-        <v>332469700</v>
+        <v>332350700</v>
       </c>
       <c r="QM35" s="4">
-        <v>-1215</v>
+        <v>-120215</v>
       </c>
       <c r="QN35" s="4">
-        <v>-100.00040903473912</v>
+        <v>-100.04047087338527</v>
       </c>
       <c r="QO35" s="4">
         <v>171498140</v>
       </c>
       <c r="QP35" s="4">
-        <v>-297042000</v>
+        <v>-297161000</v>
       </c>
     </row>
     <row r="36">
@@ -21966,10 +21966,10 @@
         <v>136874751800</v>
       </c>
       <c r="FB41" s="4">
-        <v>136873921800</v>
+        <v>134873921800</v>
       </c>
       <c r="FC41" s="4">
-        <v>-830000</v>
+        <v>-2000830000</v>
       </c>
       <c r="FD41" s="4">
         <v>0</v>
@@ -21978,7 +21978,7 @@
         <v>16037753835</v>
       </c>
       <c r="FF41" s="4">
-        <v>830000</v>
+        <v>2000830000</v>
       </c>
       <c r="FG41" s="4">
         <v>139129067300</v>
@@ -21990,19 +21990,19 @@
         <v>138158961125</v>
       </c>
       <c r="FJ41" s="4">
-        <v>138722313900</v>
+        <v>136722313900</v>
       </c>
       <c r="FK41" s="4">
-        <v>563352775</v>
+        <v>-1436647225</v>
       </c>
       <c r="FL41" s="4">
-        <v>41.92875073700051</v>
+        <v>248.09175140030422</v>
       </c>
       <c r="FM41" s="4">
         <v>199350850</v>
       </c>
       <c r="FN41" s="4">
-        <v>406753400</v>
+        <v>2406753400</v>
       </c>
       <c r="JW41" s="4">
         <v>843293000</v>
@@ -22158,10 +22158,10 @@
         <v>136874751800</v>
       </c>
       <c r="QD41" s="4">
-        <v>136873921800</v>
+        <v>134873921800</v>
       </c>
       <c r="QE41" s="4">
-        <v>-830000</v>
+        <v>-2000830000</v>
       </c>
       <c r="QF41" s="4">
         <v>0</v>
@@ -22170,7 +22170,7 @@
         <v>16037753835</v>
       </c>
       <c r="QH41" s="4">
-        <v>830000</v>
+        <v>2000830000</v>
       </c>
       <c r="QI41" s="4">
         <v>139129067300</v>
@@ -22182,19 +22182,19 @@
         <v>138158961125</v>
       </c>
       <c r="QL41" s="4">
-        <v>138722313900</v>
+        <v>136722313900</v>
       </c>
       <c r="QM41" s="4">
-        <v>563352775</v>
+        <v>-1436647225</v>
       </c>
       <c r="QN41" s="4">
-        <v>-41.92875073700051</v>
+        <v>-248.09175140030422</v>
       </c>
       <c r="QO41" s="4">
         <v>199350850</v>
       </c>
       <c r="QP41" s="4">
-        <v>-406753400</v>
+        <v>-2406753400</v>
       </c>
     </row>
     <row r="42">
@@ -22870,19 +22870,19 @@
         <v>59378475</v>
       </c>
       <c r="BB43" s="4">
-        <v>64438800</v>
+        <v>64795800</v>
       </c>
       <c r="BC43" s="4">
-        <v>5060325</v>
+        <v>5417325</v>
       </c>
       <c r="BD43" s="4">
-        <v>84.17314282899414</v>
+        <v>83.05657659855457</v>
       </c>
       <c r="BE43" s="4">
         <v>44497400</v>
       </c>
       <c r="BF43" s="4">
-        <v>26912700</v>
+        <v>26555700</v>
       </c>
       <c r="BG43" s="4">
         <v>35622400</v>
@@ -22894,19 +22894,19 @@
         <v>23154560</v>
       </c>
       <c r="BJ43" s="4">
-        <v>26191500</v>
+        <v>25775000</v>
       </c>
       <c r="BK43" s="4">
-        <v>3036940</v>
+        <v>2620440</v>
       </c>
       <c r="BL43" s="4">
-        <v>75.64181125198913</v>
+        <v>78.98240593398697</v>
       </c>
       <c r="BM43" s="4">
         <v>14787100</v>
       </c>
       <c r="BN43" s="4">
-        <v>9430900</v>
+        <v>9847400</v>
       </c>
       <c r="BO43" s="4">
         <v>45593800</v>
@@ -23038,19 +23038,19 @@
         <v>5174722528</v>
       </c>
       <c r="FJ43" s="4">
-        <v>5174720453</v>
+        <v>5174660953</v>
       </c>
       <c r="FK43" s="4">
-        <v>-2075</v>
+        <v>-61575</v>
       </c>
       <c r="FL43" s="4">
-        <v>100.00076375263139</v>
+        <v>100.02266412929026</v>
       </c>
       <c r="FM43" s="4">
         <v>165551120</v>
       </c>
       <c r="FN43" s="4">
-        <v>271686900</v>
+        <v>271746400</v>
       </c>
       <c r="KU43" s="4">
         <v>0</v>
@@ -23134,19 +23134,19 @@
         <v>59378475</v>
       </c>
       <c r="LV43" s="4">
-        <v>64438800</v>
+        <v>64795800</v>
       </c>
       <c r="LW43" s="4">
-        <v>5060325</v>
+        <v>5417325</v>
       </c>
       <c r="LX43" s="4">
-        <v>84.17314282899414</v>
+        <v>83.05657659855457</v>
       </c>
       <c r="LY43" s="4">
         <v>44497400</v>
       </c>
       <c r="LZ43" s="4">
-        <v>26912700</v>
+        <v>26555700</v>
       </c>
       <c r="MA43" s="4">
         <v>35622400</v>
@@ -23158,19 +23158,19 @@
         <v>23154560</v>
       </c>
       <c r="MD43" s="4">
-        <v>26191500</v>
+        <v>25775000</v>
       </c>
       <c r="ME43" s="4">
-        <v>3036940</v>
+        <v>2620440</v>
       </c>
       <c r="MF43" s="4">
-        <v>75.64181125198913</v>
+        <v>78.98240593398697</v>
       </c>
       <c r="MG43" s="4">
         <v>14787100</v>
       </c>
       <c r="MH43" s="4">
-        <v>9430900</v>
+        <v>9847400</v>
       </c>
       <c r="MQ43" s="4">
         <v>3445800</v>
@@ -23254,19 +23254,19 @@
         <v>5174722528</v>
       </c>
       <c r="QL43" s="4">
-        <v>5174720453</v>
+        <v>5174660953</v>
       </c>
       <c r="QM43" s="4">
-        <v>-2075</v>
+        <v>-61575</v>
       </c>
       <c r="QN43" s="4">
-        <v>-100.00076375263139</v>
+        <v>-100.02266412929026</v>
       </c>
       <c r="QO43" s="4">
         <v>165551120</v>
       </c>
       <c r="QP43" s="4">
-        <v>-271686900</v>
+        <v>-271746400</v>
       </c>
     </row>
     <row r="44">
@@ -23502,10 +23502,10 @@
         <v>4014620846</v>
       </c>
       <c r="FB44" s="4">
-        <v>4000432126</v>
+        <v>4002352926</v>
       </c>
       <c r="FC44" s="4">
-        <v>-14188720</v>
+        <v>-12267920</v>
       </c>
       <c r="FD44" s="4">
         <v>0</v>
@@ -23514,7 +23514,7 @@
         <v>1365344509</v>
       </c>
       <c r="FF44" s="4">
-        <v>14188720</v>
+        <v>12267920</v>
       </c>
       <c r="FG44" s="4">
         <v>7538481576</v>
@@ -23526,19 +23526,19 @@
         <v>5815680377.5</v>
       </c>
       <c r="FJ44" s="4">
-        <v>5801319456.5</v>
+        <v>5803240256.5</v>
       </c>
       <c r="FK44" s="4">
-        <v>-14360921</v>
+        <v>-12440121</v>
       </c>
       <c r="FL44" s="4">
-        <v>100.83357969639815</v>
+        <v>100.7220868554556</v>
       </c>
       <c r="FM44" s="4">
         <v>621843240</v>
       </c>
       <c r="FN44" s="4">
-        <v>1737162119.5</v>
+        <v>1735241319.5</v>
       </c>
       <c r="JW44" s="4">
         <v>2400720300</v>
@@ -23694,10 +23694,10 @@
         <v>4014620846</v>
       </c>
       <c r="QD44" s="4">
-        <v>4000432126</v>
+        <v>4002352926</v>
       </c>
       <c r="QE44" s="4">
-        <v>-14188720</v>
+        <v>-12267920</v>
       </c>
       <c r="QF44" s="4">
         <v>0</v>
@@ -23706,7 +23706,7 @@
         <v>1365344509</v>
       </c>
       <c r="QH44" s="4">
-        <v>14188720</v>
+        <v>12267920</v>
       </c>
       <c r="QI44" s="4">
         <v>7538481576</v>
@@ -23718,19 +23718,19 @@
         <v>5815680377.5</v>
       </c>
       <c r="QL44" s="4">
-        <v>5801319456.5</v>
+        <v>5803240256.5</v>
       </c>
       <c r="QM44" s="4">
-        <v>-14360921</v>
+        <v>-12440121</v>
       </c>
       <c r="QN44" s="4">
-        <v>-100.83357969639815</v>
+        <v>-100.7220868554556</v>
       </c>
       <c r="QO44" s="4">
         <v>621843240</v>
       </c>
       <c r="QP44" s="4">
-        <v>-1737162119.5</v>
+        <v>-1735241319.5</v>
       </c>
     </row>
     <row r="45">
@@ -26214,19 +26214,19 @@
         <v>6554070.000000002</v>
       </c>
       <c r="ET50" s="4">
-        <v>0</v>
+        <v>16947500</v>
       </c>
       <c r="EU50" s="4">
-        <v>-6554070.000000002</v>
+        <v>10393429.999999998</v>
       </c>
       <c r="EV50" s="4">
-        <v>142.8571428571429</v>
+        <v>32.03723575034837</v>
       </c>
       <c r="EW50" s="4">
         <v>0</v>
       </c>
       <c r="EX50" s="4">
-        <v>21846900</v>
+        <v>4899400</v>
       </c>
       <c r="EY50" s="4">
         <v>1161510811</v>
@@ -26238,10 +26238,10 @@
         <v>1161510811</v>
       </c>
       <c r="FB50" s="4">
-        <v>1161510811</v>
+        <v>1172698211</v>
       </c>
       <c r="FC50" s="4">
-        <v>0</v>
+        <v>11187400</v>
       </c>
       <c r="FD50" s="4">
         <v>0</v>
@@ -26250,7 +26250,7 @@
         <v>408871876</v>
       </c>
       <c r="FF50" s="4">
-        <v>0</v>
+        <v>-11187400</v>
       </c>
       <c r="FG50" s="4">
         <v>1389436011</v>
@@ -26262,19 +26262,19 @@
         <v>1288243226</v>
       </c>
       <c r="FJ50" s="4">
-        <v>1267278811</v>
+        <v>1295413711</v>
       </c>
       <c r="FK50" s="4">
-        <v>-20964415</v>
+        <v>7170485</v>
       </c>
       <c r="FL50" s="4">
-        <v>120.71730212781475</v>
+        <v>92.91403532376344</v>
       </c>
       <c r="FM50" s="4">
         <v>14690500</v>
       </c>
       <c r="FN50" s="4">
-        <v>122157200</v>
+        <v>94022300</v>
       </c>
       <c r="KM50" s="4">
         <v>73250000</v>
@@ -26406,10 +26406,10 @@
         <v>1161510811</v>
       </c>
       <c r="QD50" s="4">
-        <v>1161510811</v>
+        <v>1172698211</v>
       </c>
       <c r="QE50" s="4">
-        <v>0</v>
+        <v>11187400</v>
       </c>
       <c r="QF50" s="4">
         <v>0</v>
@@ -26418,7 +26418,7 @@
         <v>408871876</v>
       </c>
       <c r="QH50" s="4">
-        <v>0</v>
+        <v>-11187400</v>
       </c>
       <c r="QI50" s="4">
         <v>1389436011</v>
@@ -26430,19 +26430,19 @@
         <v>1288243226</v>
       </c>
       <c r="QL50" s="4">
-        <v>1267278811</v>
+        <v>1295413711</v>
       </c>
       <c r="QM50" s="4">
-        <v>-20964415</v>
+        <v>7170485</v>
       </c>
       <c r="QN50" s="4">
-        <v>-120.71730212781475</v>
+        <v>-92.91403532376344</v>
       </c>
       <c r="QO50" s="4">
         <v>14690500</v>
       </c>
       <c r="QP50" s="4">
-        <v>-122157200</v>
+        <v>-94022300</v>
       </c>
     </row>
     <row r="51">

</xml_diff>